<commit_message>
Updated spreadsheet with sshd changes.
</commit_message>
<xml_diff>
--- a/rhel9-cis-benchmarks_1-0-0.xlsx
+++ b/rhel9-cis-benchmarks_1-0-0.xlsx
@@ -997,7 +997,7 @@
     <t>5.2.4 Ensure SSH access is limited (Automated)</t>
   </si>
   <si>
-    <t>Inserted ‘AllowGroups sshusers’ into /etc/ssh/sshd_config. Created ‘sshusers’ group. User accounts requiring ssh access must be added to this group.</t>
+    <t>Updated /etc/ssh/sshd_config.d/00-complianceascode-hardening.conf. Created ‘sshusers’ group. User accounts requiring ssh access must be added to this group.</t>
   </si>
   <si>
     <t>5.2.5 Ensure SSH LogLevel is appropriate (Automated)</t>
@@ -1036,7 +1036,7 @@
     <t>5.2.15 Ensure SSH warning banner is configured (Automated)</t>
   </si>
   <si>
-    <t>Set ‘Banner /etc/issue’ in /etc/ssh/sshd_conf</t>
+    <t>Updated /etc/ssh/sshd_config.d/00-complianceascode-hardening.conf. Set ‘Banner /etc/issue’.</t>
   </si>
   <si>
     <t>5.2.16 Ensure SSH MaxAuthTries is set to 4 or less (Automated)</t>
@@ -1054,7 +1054,7 @@
     <t>5.2.20 Ensure SSH Idle Timeout Interval is configured (Automated)</t>
   </si>
   <si>
-    <t>Set ‘ClientAliveInterval 3540’ and ‘ClientAliveCountMax 0’ in /etc/ssh/sshd_config in accordance with organization 60 minute timeout policy.</t>
+    <t>Updated /etc/ssh/sshd_config.d/00-complianceascode-hardening.conf. Set ‘ClientAliveInterval 3540’ and ‘ClientAliveCountMax 0’ in accordance with organization 60 minute timeout policy.</t>
   </si>
   <si>
     <t>5.3 Configure privilege escalation</t>
@@ -1646,7 +1646,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="ff000000"/>
@@ -1688,50 +1688,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="15"/>
           <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="15"/>
-          <bgColor indexed="16"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="15"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="15"/>
-          <bgColor indexed="19"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="15"/>
-          <bgColor indexed="18"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5279,7 +5235,7 @@
   <cols>
     <col min="1" max="1" width="89.6719" style="32" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="32" customWidth="1"/>
-    <col min="3" max="3" width="45.7969" style="32" customWidth="1"/>
+    <col min="3" max="3" width="45.8516" style="32" customWidth="1"/>
     <col min="4" max="4" width="57.1719" style="32" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="32" customWidth="1"/>
     <col min="6" max="16384" width="16.3516" style="32" customWidth="1"/>
@@ -6113,7 +6069,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B21 B35:B67">
+  <conditionalFormatting sqref="B2:B68">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Pass"</formula>
     </cfRule>
@@ -6124,20 +6080,6 @@
       <formula>"Remediated"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="15" priority="4" operator="equal" stopIfTrue="1">
-      <formula>"Alternate"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:B34 B68">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal" stopIfTrue="1">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal" stopIfTrue="1">
-      <formula>"Fail"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal" stopIfTrue="1">
-      <formula>"Remediated"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal" stopIfTrue="1">
       <formula>"Alternate"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6556,7 +6498,7 @@
         <v>313</v>
       </c>
       <c r="B28" t="s" s="14">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="C28" s="16"/>
       <c r="D28" t="s" s="15">
@@ -7044,16 +6986,16 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B61">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal" stopIfTrue="1">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal" stopIfTrue="1">
       <formula>"Alternate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal" stopIfTrue="1">
       <formula>"Remediated"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7582,16 +7524,16 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B35">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal" stopIfTrue="1">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal" stopIfTrue="1">
       <formula>"Alternate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal" stopIfTrue="1">
       <formula>"Remediated"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>